<commit_message>
Updated plate files with new changes to src010 and P3643
</commit_message>
<xml_diff>
--- a/crisscross_kit/crisscross/dna_source_plates/seed_plates/P3643_MA_combined_seeds_8064.xlsx
+++ b/crisscross_kit/crisscross/dna_source_plates/seed_plates/P3643_MA_combined_seeds_8064.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/Shih_Lab_Postdoc/research_projects/crisscross_code/crisscross_kit/crisscross/dna_source_plates/seed_plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C10030-7126-6840-9F75-74D9F3257B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91259E1B-197D-7C44-A3D1-CAEF0E476015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="51200" windowHeight="28180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="1151">
   <si>
     <t>well</t>
   </si>
@@ -2758,6 +2758,726 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>SEED-1_1-h2-position_6</t>
+  </si>
+  <si>
+    <t>GAAACAATCGGCAAGAGACGCAGAAACAGCCGCACAGGCGGCttTTCATTAAAG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 6, Side h2, 8064 Seed ID 1_1</t>
+  </si>
+  <si>
+    <t>SEED-2_1-h2-position_7</t>
+  </si>
+  <si>
+    <t>AAGCGCCATTCGGCAAGGCGATTAAGTTGGATAACCTCACCGttAAGACACCAC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 7, Side h2, 8064 Seed ID 2_1</t>
+  </si>
+  <si>
+    <t>SEED-3_1-h2-position_8</t>
+  </si>
+  <si>
+    <t>TCAACATTAAATGGCGCATCGTAACCGTGCGGAAACCAGGCAttTGCTTCTGTA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 8, Side h2, 8064 Seed ID 3_1</t>
+  </si>
+  <si>
+    <t>SEED-4_1-h2-position_9</t>
+  </si>
+  <si>
+    <t>TCGTAAAACTAGCGTTAATATTTTGTTAAAAGCCAGCTTTCAttCCTGAGCAAA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 9, Side h2, 8064 Seed ID 4_1</t>
+  </si>
+  <si>
+    <t>SEED-5_1-h2-position_10</t>
+  </si>
+  <si>
+    <t>TATTTTAAATGCCGTTCTAGCTGATAAATTGATGAACGGTAAttAGCACTAAAT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 10, Side h2, 8064 Seed ID 5_1</t>
+  </si>
+  <si>
+    <t>SEED-1_9-h2-position_6</t>
+  </si>
+  <si>
+    <t>GAAACAATCGGCAAGAGACGCAGAAACAGCCGCACAGGCGGCttCCACCAGAAC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 6, Side h2, 8064 Seed ID 1_9</t>
+  </si>
+  <si>
+    <t>SEED-2_9-h2-position_7</t>
+  </si>
+  <si>
+    <t>AAGCGCCATTCGGCAAGGCGATTAAGTTGGATAACCTCACCGttAAAACAGGGA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 7, Side h2, 8064 Seed ID 2_9</t>
+  </si>
+  <si>
+    <t>SEED-3_9-h2-position_8</t>
+  </si>
+  <si>
+    <t>TCAACATTAAATGGCGCATCGTAACCGTGCGGAAACCAGGCAttAAAGCCTGTT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 8, Side h2, 8064 Seed ID 3_9</t>
+  </si>
+  <si>
+    <t>SEED-4_9-h2-position_9</t>
+  </si>
+  <si>
+    <t>TCGTAAAACTAGCGTTAATATTTTGTTAAAAGCCAGCTTTCAttAAGTTTGAGT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 9, Side h2, 8064 Seed ID 4_9</t>
+  </si>
+  <si>
+    <t>SEED-5_9-h2-position_10</t>
+  </si>
+  <si>
+    <t>TATTTTAAATGCCGTTCTAGCTGATAAATTGATGAACGGTAAttAAAGAGTCTG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 10, Side h2, 8064 Seed ID 5_9</t>
+  </si>
+  <si>
+    <t>SEED-1_2-h2-position_27</t>
+  </si>
+  <si>
+    <t>TAGCAAGCAAATAATCAAGATTAGTTGCTAAAACAGCCATATttTGGGAATTAG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 27, Side h2, 8064 Seed ID 1_2</t>
+  </si>
+  <si>
+    <t>SEED-2_2-h2-position_26</t>
+  </si>
+  <si>
+    <t>TATTTATCCCAAGCATTAGACGGGAGAATTATAAGAGCAAGAttGAAAATACAT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 26, Side h2, 8064 Seed ID 2_2</t>
+  </si>
+  <si>
+    <t>SEED-3_2-h2-position_25</t>
+  </si>
+  <si>
+    <t>AACAATGAAATAAATAATAACGGAATACCCAAAGAAACGCAAttTCCTTGAAAA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 25, Side h2, 8064 Seed ID 3_2</t>
+  </si>
+  <si>
+    <t>SEED-4_2-h2-position_24</t>
+  </si>
+  <si>
+    <t>AGACACCACGGAGGAGGGAAGGTAAATATTCACCATTACCATttAAGTTACAAA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 24, Side h2, 8064 Seed ID 4_2</t>
+  </si>
+  <si>
+    <t>SEED-5_2-h2-position_23</t>
+  </si>
+  <si>
+    <t>TAGCAAGGCCGGCGTTTTCATCGGCATTTTCAGAGCCGCCACttTTGACGGGGA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 23, Side h2, 8064 Seed ID 5_2</t>
+  </si>
+  <si>
+    <t>SEED-1_3-h2-position_6</t>
+  </si>
+  <si>
+    <t>GAAACAATCGGCAAGAGACGCAGAAACAGCCGCACAGGCGGCttTTAGCAAGGC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 6, Side h2, 8064 Seed ID 1_3</t>
+  </si>
+  <si>
+    <t>SEED-2_3-h2-position_7</t>
+  </si>
+  <si>
+    <t>AAGCGCCATTCGGCAAGGCGATTAAGTTGGATAACCTCACCGttCATGATTAAG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 7, Side h2, 8064 Seed ID 2_3</t>
+  </si>
+  <si>
+    <t>SEED-3_3-h2-position_8</t>
+  </si>
+  <si>
+    <t>TCAACATTAAATGGCGCATCGTAACCGTGCGGAAACCAGGCAttGAGTCAATAG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 8, Side h2, 8064 Seed ID 3_3</t>
+  </si>
+  <si>
+    <t>SEED-4_3-h2-position_9</t>
+  </si>
+  <si>
+    <t>TCGTAAAACTAGCGTTAATATTTTGTTAAAAGCCAGCTTTCAttCGGGAGAAAC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 9, Side h2, 8064 Seed ID 4_3</t>
+  </si>
+  <si>
+    <t>SEED-5_3-h2-position_10</t>
+  </si>
+  <si>
+    <t>TATTTTAAATGCCGTTCTAGCTGATAAATTGATGAACGGTAAttGAAAGCGAAA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 10, Side h2, 8064 Seed ID 5_3</t>
+  </si>
+  <si>
+    <t>SEED-1_4-h2-position_27</t>
+  </si>
+  <si>
+    <t>TAGCAAGCAAATAATCAAGATTAGTTGCTAAAACAGCCATATttGCACCGTAAT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 27, Side h2, 8064 Seed ID 1_4</t>
+  </si>
+  <si>
+    <t>SEED-2_4-h2-position_26</t>
+  </si>
+  <si>
+    <t>TATTTATCCCAAGCATTAGACGGGAGAATTATAAGAGCAAGAttACCGAGGAAA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 26, Side h2, 8064 Seed ID 2_4</t>
+  </si>
+  <si>
+    <t>SEED-3_4-h2-position_25</t>
+  </si>
+  <si>
+    <t>AACAATGAAATAAATAATAACGGAATACCCAAAGAAACGCAAttACCTTTTTAA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 25, Side h2, 8064 Seed ID 3_4</t>
+  </si>
+  <si>
+    <t>SEED-4_4-h2-position_24</t>
+  </si>
+  <si>
+    <t>AGACACCACGGAGGAGGGAAGGTAAATATTCACCATTACCATttGTTTAACGTC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 24, Side h2, 8064 Seed ID 4_4</t>
+  </si>
+  <si>
+    <t>SEED-5_4-h2-position_23</t>
+  </si>
+  <si>
+    <t>TAGCAAGGCCGGCGTTTTCATCGGCATTTTCAGAGCCGCCACttGGTCACGCTG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 23, Side h2, 8064 Seed ID 5_4</t>
+  </si>
+  <si>
+    <t>SEED-1_5-h2-position_6</t>
+  </si>
+  <si>
+    <t>GAAACAATCGGCAAGAGACGCAGAAACAGCCGCACAGGCGGCttTCAGACTGTA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 6, Side h2, 8064 Seed ID 1_5</t>
+  </si>
+  <si>
+    <t>SEED-2_5-h2-position_7</t>
+  </si>
+  <si>
+    <t>AAGCGCCATTCGGCAAGGCGATTAAGTTGGATAACCTCACCGttAAGAAAAGTA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 7, Side h2, 8064 Seed ID 2_5</t>
+  </si>
+  <si>
+    <t>SEED-3_5-h2-position_8</t>
+  </si>
+  <si>
+    <t>TCAACATTAAATGGCGCATCGTAACCGTGCGGAAACCAGGCAttGTAAATGCTG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 8, Side h2, 8064 Seed ID 3_5</t>
+  </si>
+  <si>
+    <t>SEED-4_5-h2-position_9</t>
+  </si>
+  <si>
+    <t>TCGTAAAACTAGCGTTAATATTTTGTTAAAAGCCAGCTTTCAttTTGCACGTAA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 9, Side h2, 8064 Seed ID 4_5</t>
+  </si>
+  <si>
+    <t>SEED-5_5-h2-position_10</t>
+  </si>
+  <si>
+    <t>TATTTTAAATGCCGTTCTAGCTGATAAATTGATGAACGGTAAttGCCGCTACAG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 10, Side h2, 8064 Seed ID 5_5</t>
+  </si>
+  <si>
+    <t>SEED-1_6-h2-position_27</t>
+  </si>
+  <si>
+    <t>TAGCAAGCAAATAATCAAGATTAGTTGCTAAAACAGCCATATttCCCTTATTAG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 27, Side h2, 8064 Seed ID 1_6</t>
+  </si>
+  <si>
+    <t>SEED-2_6-h2-position_26</t>
+  </si>
+  <si>
+    <t>TATTTATCCCAAGCATTAGACGGGAGAATTATAAGAGCAAGAttAAACAATGAA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 26, Side h2, 8064 Seed ID 2_6</t>
+  </si>
+  <si>
+    <t>SEED-3_6-h2-position_25</t>
+  </si>
+  <si>
+    <t>AACAATGAAATAAATAATAACGGAATACCCAAAGAAACGCAAttGAAAACTTTT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 25, Side h2, 8064 Seed ID 3_6</t>
+  </si>
+  <si>
+    <t>SEED-4_6-h2-position_24</t>
+  </si>
+  <si>
+    <t>AGACACCACGGAGGAGGGAAGGTAAATATTCACCATTACCATttTCTGAATAAT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 24, Side h2, 8064 Seed ID 4_6</t>
+  </si>
+  <si>
+    <t>SEED-5_6-h2-position_23</t>
+  </si>
+  <si>
+    <t>TAGCAAGGCCGGCGTTTTCATCGGCATTTTCAGAGCCGCCACttATAACGTGCT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 23, Side h2, 8064 Seed ID 5_6</t>
+  </si>
+  <si>
+    <t>SEED-1_7-h2-position_6</t>
+  </si>
+  <si>
+    <t>GAAACAATCGGCAAGAGACGCAGAAACAGCCGCACAGGCGGCttGAACCAGAGC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 6, Side h2, 8064 Seed ID 1_7</t>
+  </si>
+  <si>
+    <t>SEED-2_7-h2-position_7</t>
+  </si>
+  <si>
+    <t>AAGCGCCATTCGGCAAGGCGATTAAGTTGGATAACCTCACCGttATAACCCACA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 7, Side h2, 8064 Seed ID 2_7</t>
+  </si>
+  <si>
+    <t>SEED-3_7-h2-position_8</t>
+  </si>
+  <si>
+    <t>TCAACATTAAATGGCGCATCGTAACCGTGCGGAAACCAGGCAttCCTAAATTTA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 8, Side h2, 8064 Seed ID 3_7</t>
+  </si>
+  <si>
+    <t>SEED-4_7-h2-position_9</t>
+  </si>
+  <si>
+    <t>TCGTAAAACTAGCGTTAATATTTTGTTAAAAGCCAGCTTTCAttATGGCAATTC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 9, Side h2, 8064 Seed ID 4_7</t>
+  </si>
+  <si>
+    <t>SEED-5_7-h2-position_10</t>
+  </si>
+  <si>
+    <t>TATTTTAAATGCCGTTCTAGCTGATAAATTGATGAACGGTAAttGGAGGCCGAT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 10, Side h2, 8064 Seed ID 5_7</t>
+  </si>
+  <si>
+    <t>SEED-1_8-h2-position_27</t>
+  </si>
+  <si>
+    <t>TAGCAAGCAAATAATCAAGATTAGTTGCTAAAACAGCCATATttCCCTCAGAAC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 27, Side h2, 8064 Seed ID 1_8</t>
+  </si>
+  <si>
+    <t>SEED-2_8-h2-position_26</t>
+  </si>
+  <si>
+    <t>TATTTATCCCAAGCATTAGACGGGAGAATTATAAGAGCAAGAttCTGAACAAAG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 26, Side h2, 8064 Seed ID 2_8</t>
+  </si>
+  <si>
+    <t>SEED-3_8-h2-position_25</t>
+  </si>
+  <si>
+    <t>AACAATGAAATAAATAATAACGGAATACCCAAAGAAACGCAAttGGCGTTAAAT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 25, Side h2, 8064 Seed ID 3_8</t>
+  </si>
+  <si>
+    <t>SEED-4_8-h2-position_24</t>
+  </si>
+  <si>
+    <t>AGACACCACGGAGGAGGGAAGGTAAATATTCACCATTACCATttCAGAAGGAGC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 24, Side h2, 8064 Seed ID 4_8</t>
+  </si>
+  <si>
+    <t>SEED-5_8-h2-position_23</t>
+  </si>
+  <si>
+    <t>TAGCAAGGCCGGCGTTTTCATCGGCATTTTCAGAGCCGCCACttAATCCTGAGA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 23, Side h2, 8064 Seed ID 5_8</t>
+  </si>
+  <si>
+    <t>SEED-1_10-h2-position_27</t>
+  </si>
+  <si>
+    <t>TAGCAAGCAAATAATCAAGATTAGTTGCTAAAACAGCCATATttGGTTGAGGCA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 27, Side h2, 8064 Seed ID 1_10</t>
+  </si>
+  <si>
+    <t>SEED-2_10-h2-position_26</t>
+  </si>
+  <si>
+    <t>TATTTATCCCAAGCATTAGACGGGAGAATTATAAGAGCAAGAttGTCAAAAATG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 26, Side h2, 8064 Seed ID 2_10</t>
+  </si>
+  <si>
+    <t>SEED-3_10-h2-position_25</t>
+  </si>
+  <si>
+    <t>AACAATGAAATAAATAATAACGGAATACCCAAAGAAACGCAAttGTATAAAGCC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 25, Side h2, 8064 Seed ID 3_10</t>
+  </si>
+  <si>
+    <t>SEED-4_10-h2-position_24</t>
+  </si>
+  <si>
+    <t>AGACACCACGGAGGAGGGAAGGTAAATATTCACCATTACCATttCAACTCGTAT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 24, Side h2, 8064 Seed ID 4_10</t>
+  </si>
+  <si>
+    <t>SEED-5_10-h2-position_23</t>
+  </si>
+  <si>
+    <t>TAGCAAGGCCGGCGTTTTCATCGGCATTTTCAGAGCCGCCACttTTCTTTGATT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 23, Side h2, 8064 Seed ID 5_10</t>
+  </si>
+  <si>
+    <t>SEED-1_11-h2-position_6</t>
+  </si>
+  <si>
+    <t>GAAACAATCGGCAAGAGACGCAGAAACAGCCGCACAGGCGGCttAATAAATCCT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 6, Side h2, 8064 Seed ID 1_11</t>
+  </si>
+  <si>
+    <t>SEED-2_11-h2-position_7</t>
+  </si>
+  <si>
+    <t>AAGCGCCATTCGGCAAGGCGATTAAGTTGGATAACCTCACCGttTTATTTATCC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 7, Side h2, 8064 Seed ID 2_11</t>
+  </si>
+  <si>
+    <t>SEED-3_11-h2-position_8</t>
+  </si>
+  <si>
+    <t>TCAACATTAAATGGCGCATCGTAACCGTGCGGAAACCAGGCAttCCATATTTAA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 8, Side h2, 8064 Seed ID 3_11</t>
+  </si>
+  <si>
+    <t>SEED-4_11-h2-position_9</t>
+  </si>
+  <si>
+    <t>TCGTAAAACTAGCGTTAATATTTTGTTAAAAGCCAGCTTTCAttCATTTGAGGA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 9, Side h2, 8064 Seed ID 4_11</t>
+  </si>
+  <si>
+    <t>SEED-5_11-h2-position_10</t>
+  </si>
+  <si>
+    <t>TATTTTAAATGCCGTTCTAGCTGATAAATTGATGAACGGTAAttTCAAACTATC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 10, Side h2, 8064 Seed ID 5_11</t>
+  </si>
+  <si>
+    <t>SEED-1_12-h2-position_27</t>
+  </si>
+  <si>
+    <t>TAGCAAGCAAATAATCAAGATTAGTTGCTAAAACAGCCATATttAATTTACCGT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 27, Side h2, 8064 Seed ID 1_12</t>
+  </si>
+  <si>
+    <t>SEED-2_12-h2-position_26</t>
+  </si>
+  <si>
+    <t>TATTTATCCCAAGCATTAGACGGGAGAATTATAAGAGCAAGAttTTTCCAGAGC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 26, Side h2, 8064 Seed ID 2_12</t>
+  </si>
+  <si>
+    <t>SEED-3_12-h2-position_25</t>
+  </si>
+  <si>
+    <t>AACAATGAAATAAATAATAACGGAATACCCAAAGAAACGCAAttTTCGAGCCAG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 25, Side h2, 8064 Seed ID 3_12</t>
+  </si>
+  <si>
+    <t>SEED-4_12-h2-position_24</t>
+  </si>
+  <si>
+    <t>AGACACCACGGAGGAGGGAAGGTAAATATTCACCATTACCATttGAGCACTAAC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 24, Side h2, 8064 Seed ID 4_12</t>
+  </si>
+  <si>
+    <t>SEED-5_12-h2-position_23</t>
+  </si>
+  <si>
+    <t>TAGCAAGGCCGGCGTTTTCATCGGCATTTTCAGAGCCGCCACttCGCCAGCCAT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 23, Side h2, 8064 Seed ID 5_12</t>
+  </si>
+  <si>
+    <t>SEED-1_13-h2-position_6</t>
+  </si>
+  <si>
+    <t>GAAACAATCGGCAAGAGACGCAGAAACAGCCGCACAGGCGGCttACAGGAGTGT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 6, Side h2, 8064 Seed ID 1_13</t>
+  </si>
+  <si>
+    <t>SEED-2_13-h2-position_7</t>
+  </si>
+  <si>
+    <t>AAGCGCCATTCGGCAAGGCGATTAAGTTGGATAACCTCACCGttGCTACAATTT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 7, Side h2, 8064 Seed ID 2_13</t>
+  </si>
+  <si>
+    <t>SEED-3_13-h2-position_8</t>
+  </si>
+  <si>
+    <t>TCAACATTAAATGGCGCATCGTAACCGTGCGGAAACCAGGCAttAAAGTAATTC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 8, Side h2, 8064 Seed ID 3_13</t>
+  </si>
+  <si>
+    <t>SEED-4_13-h2-position_9</t>
+  </si>
+  <si>
+    <t>TCGTAAAACTAGCGTTAATATTTTGTTAAAAGCCAGCTTTCAttCAGTTGAAAG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 9, Side h2, 8064 Seed ID 4_13</t>
+  </si>
+  <si>
+    <t>SEED-5_13-h2-position_10</t>
+  </si>
+  <si>
+    <t>TATTTTAAATGCCGTTCTAGCTGATAAATTGATGAACGGTAAttCATTTTGACG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 10, Side h2, 8064 Seed ID 5_13</t>
+  </si>
+  <si>
+    <t>SEED-1_14-h2-position_27</t>
+  </si>
+  <si>
+    <t>TAGCAAGCAAATAATCAAGATTAGTTGCTAAAACAGCCATATttTGAGTAACAG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 27, Side h2, 8064 Seed ID 1_14</t>
+  </si>
+  <si>
+    <t>SEED-2_14-h2-position_26</t>
+  </si>
+  <si>
+    <t>TATTTATCCCAAGCATTAGACGGGAGAATTATAAGAGCAAGAttTTTTGAAGCC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 26, Side h2, 8064 Seed ID 2_14</t>
+  </si>
+  <si>
+    <t>SEED-3_14-h2-position_25</t>
+  </si>
+  <si>
+    <t>AACAATGAAATAAATAATAACGGAATACCCAAAGAAACGCAAttGCTAATGCAG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 25, Side h2, 8064 Seed ID 3_14</t>
+  </si>
+  <si>
+    <t>SEED-4_14-h2-position_24</t>
+  </si>
+  <si>
+    <t>AGACACCACGGAGGAGGGAAGGTAAATATTCACCATTACCATttATATCAAACC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 24, Side h2, 8064 Seed ID 4_14</t>
+  </si>
+  <si>
+    <t>SEED-5_14-h2-position_23</t>
+  </si>
+  <si>
+    <t>TAGCAAGGCCGGCGTTTTCATCGGCATTTTCAGAGCCGCCACttCAGATTCACC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 23, Side h2, 8064 Seed ID 5_14</t>
+  </si>
+  <si>
+    <t>SEED-1_15-h2-position_6</t>
+  </si>
+  <si>
+    <t>GAAACAATCGGCAAGAGACGCAGAAACAGCCGCACAGGCGGCttTTTCGGAACC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 6, Side h2, 8064 Seed ID 1_15</t>
+  </si>
+  <si>
+    <t>SEED-2_15-h2-position_7</t>
+  </si>
+  <si>
+    <t>AAGCGCCATTCGGCAAGGCGATTAAGTTGGATAACCTCACCGttAGAACGCGAG</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 7, Side h2, 8064 Seed ID 2_15</t>
+  </si>
+  <si>
+    <t>SEED-3_15-h2-position_8</t>
+  </si>
+  <si>
+    <t>TCAACATTAAATGGCGCATCGTAACCGTGCGGAAACCAGGCAttTGAACAAGAA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 8, Side h2, 8064 Seed ID 3_15</t>
+  </si>
+  <si>
+    <t>SEED-4_15-h2-position_9</t>
+  </si>
+  <si>
+    <t>TCGTAAAACTAGCGTTAATATTTTGTTAAAAGCCAGCTTTCAttCAGCAAATGA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 9, Side h2, 8064 Seed ID 4_15</t>
+  </si>
+  <si>
+    <t>SEED-5_15-h2-position_10</t>
+  </si>
+  <si>
+    <t>TATTTTAAATGCCGTTCTAGCTGATAAATTGATGAACGGTAAttGGCCAACAGA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 10, Side h2, 8064 Seed ID 5_15</t>
+  </si>
+  <si>
+    <t>SEED-1_16-h2-position_27</t>
+  </si>
+  <si>
+    <t>TAGCAAGCAAATAATCAAGATTAGTTGCTAAAACAGCCATATttTGAGACTCCT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 27, Side h2, 8064 Seed ID 1_16</t>
+  </si>
+  <si>
+    <t>SEED-2_16-h2-position_26</t>
+  </si>
+  <si>
+    <t>TATTTATCCCAAGCATTAGACGGGAGAATTATAAGAGCAAGAttATAGCAAGCA</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 26, Side h2, 8064 Seed ID 2_16</t>
+  </si>
+  <si>
+    <t>SEED-3_16-h2-position_25</t>
+  </si>
+  <si>
+    <t>AACAATGAAATAAATAATAACGGAATACCCAAAGAAACGCAAttAGAAACCAAT</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 25, Side h2, 8064 Seed ID 3_16</t>
+  </si>
+  <si>
+    <t>SEED-4_16-h2-position_24</t>
+  </si>
+  <si>
+    <t>AGACACCACGGAGGAGGGAAGGTAAATATTCACCATTACCATttCAGTATTAAC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 24, Side h2, 8064 Seed ID 4_16</t>
+  </si>
+  <si>
+    <t>SEED-5_16-h2-position_23</t>
+  </si>
+  <si>
+    <t>TAGCAAGGCCGGCGTTTTCATCGGCATTTTCAGAGCCGCCACttTACGTGGCAC</t>
+  </si>
+  <si>
+    <t>Seed Handle For Slat Position 23, Side h2, 8064 Seed ID 5_16</t>
   </si>
 </sst>
 </file>
@@ -3141,15 +3861,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E385"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView zoomScale="142" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="3" width="56.6640625" customWidth="1"/>
+    <col min="3" max="3" width="68" customWidth="1"/>
     <col min="4" max="4" width="62.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
@@ -3355,26 +4075,86 @@
       <c r="A14" t="s">
         <v>17</v>
       </c>
+      <c r="B14" t="s">
+        <v>911</v>
+      </c>
+      <c r="C14" t="s">
+        <v>912</v>
+      </c>
+      <c r="D14" t="s">
+        <v>913</v>
+      </c>
+      <c r="E14">
+        <v>200</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
+      <c r="B15" t="s">
+        <v>914</v>
+      </c>
+      <c r="C15" t="s">
+        <v>915</v>
+      </c>
+      <c r="D15" t="s">
+        <v>916</v>
+      </c>
+      <c r="E15">
+        <v>200</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
+      <c r="B16" t="s">
+        <v>917</v>
+      </c>
+      <c r="C16" t="s">
+        <v>918</v>
+      </c>
+      <c r="D16" t="s">
+        <v>919</v>
+      </c>
+      <c r="E16">
+        <v>200</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
+      <c r="B17" t="s">
+        <v>920</v>
+      </c>
+      <c r="C17" t="s">
+        <v>921</v>
+      </c>
+      <c r="D17" t="s">
+        <v>922</v>
+      </c>
+      <c r="E17">
+        <v>200</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
+      <c r="B18" t="s">
+        <v>923</v>
+      </c>
+      <c r="C18" t="s">
+        <v>924</v>
+      </c>
+      <c r="D18" t="s">
+        <v>925</v>
+      </c>
+      <c r="E18">
+        <v>200</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -3595,26 +4375,86 @@
       <c r="A38" t="s">
         <v>41</v>
       </c>
+      <c r="B38" t="s">
+        <v>941</v>
+      </c>
+      <c r="C38" t="s">
+        <v>942</v>
+      </c>
+      <c r="D38" t="s">
+        <v>943</v>
+      </c>
+      <c r="E38">
+        <v>200</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
+      <c r="B39" t="s">
+        <v>944</v>
+      </c>
+      <c r="C39" t="s">
+        <v>945</v>
+      </c>
+      <c r="D39" t="s">
+        <v>946</v>
+      </c>
+      <c r="E39">
+        <v>200</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>43</v>
       </c>
+      <c r="B40" t="s">
+        <v>947</v>
+      </c>
+      <c r="C40" t="s">
+        <v>948</v>
+      </c>
+      <c r="D40" t="s">
+        <v>949</v>
+      </c>
+      <c r="E40">
+        <v>200</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>44</v>
       </c>
+      <c r="B41" t="s">
+        <v>950</v>
+      </c>
+      <c r="C41" t="s">
+        <v>951</v>
+      </c>
+      <c r="D41" t="s">
+        <v>952</v>
+      </c>
+      <c r="E41">
+        <v>200</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>45</v>
       </c>
+      <c r="B42" t="s">
+        <v>953</v>
+      </c>
+      <c r="C42" t="s">
+        <v>954</v>
+      </c>
+      <c r="D42" t="s">
+        <v>955</v>
+      </c>
+      <c r="E42">
+        <v>200</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -3835,26 +4675,86 @@
       <c r="A62" t="s">
         <v>65</v>
       </c>
+      <c r="B62" t="s">
+        <v>956</v>
+      </c>
+      <c r="C62" t="s">
+        <v>957</v>
+      </c>
+      <c r="D62" t="s">
+        <v>958</v>
+      </c>
+      <c r="E62">
+        <v>200</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>66</v>
       </c>
+      <c r="B63" t="s">
+        <v>959</v>
+      </c>
+      <c r="C63" t="s">
+        <v>960</v>
+      </c>
+      <c r="D63" t="s">
+        <v>961</v>
+      </c>
+      <c r="E63">
+        <v>200</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>67</v>
       </c>
+      <c r="B64" t="s">
+        <v>962</v>
+      </c>
+      <c r="C64" t="s">
+        <v>963</v>
+      </c>
+      <c r="D64" t="s">
+        <v>964</v>
+      </c>
+      <c r="E64">
+        <v>200</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>68</v>
       </c>
+      <c r="B65" t="s">
+        <v>965</v>
+      </c>
+      <c r="C65" t="s">
+        <v>966</v>
+      </c>
+      <c r="D65" t="s">
+        <v>967</v>
+      </c>
+      <c r="E65">
+        <v>200</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>69</v>
       </c>
+      <c r="B66" t="s">
+        <v>968</v>
+      </c>
+      <c r="C66" t="s">
+        <v>969</v>
+      </c>
+      <c r="D66" t="s">
+        <v>970</v>
+      </c>
+      <c r="E66">
+        <v>200</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
@@ -4075,26 +4975,86 @@
       <c r="A86" t="s">
         <v>89</v>
       </c>
+      <c r="B86" t="s">
+        <v>971</v>
+      </c>
+      <c r="C86" t="s">
+        <v>972</v>
+      </c>
+      <c r="D86" t="s">
+        <v>973</v>
+      </c>
+      <c r="E86">
+        <v>200</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>90</v>
       </c>
+      <c r="B87" t="s">
+        <v>974</v>
+      </c>
+      <c r="C87" t="s">
+        <v>975</v>
+      </c>
+      <c r="D87" t="s">
+        <v>976</v>
+      </c>
+      <c r="E87">
+        <v>200</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>91</v>
       </c>
+      <c r="B88" t="s">
+        <v>977</v>
+      </c>
+      <c r="C88" t="s">
+        <v>978</v>
+      </c>
+      <c r="D88" t="s">
+        <v>979</v>
+      </c>
+      <c r="E88">
+        <v>200</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>92</v>
       </c>
+      <c r="B89" t="s">
+        <v>980</v>
+      </c>
+      <c r="C89" t="s">
+        <v>981</v>
+      </c>
+      <c r="D89" t="s">
+        <v>982</v>
+      </c>
+      <c r="E89">
+        <v>200</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>93</v>
       </c>
+      <c r="B90" t="s">
+        <v>983</v>
+      </c>
+      <c r="C90" t="s">
+        <v>984</v>
+      </c>
+      <c r="D90" t="s">
+        <v>985</v>
+      </c>
+      <c r="E90">
+        <v>200</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
@@ -4315,26 +5275,86 @@
       <c r="A110" t="s">
         <v>113</v>
       </c>
+      <c r="B110" t="s">
+        <v>986</v>
+      </c>
+      <c r="C110" t="s">
+        <v>987</v>
+      </c>
+      <c r="D110" t="s">
+        <v>988</v>
+      </c>
+      <c r="E110">
+        <v>200</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>114</v>
       </c>
+      <c r="B111" t="s">
+        <v>989</v>
+      </c>
+      <c r="C111" t="s">
+        <v>990</v>
+      </c>
+      <c r="D111" t="s">
+        <v>991</v>
+      </c>
+      <c r="E111">
+        <v>200</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>115</v>
       </c>
+      <c r="B112" t="s">
+        <v>992</v>
+      </c>
+      <c r="C112" t="s">
+        <v>993</v>
+      </c>
+      <c r="D112" t="s">
+        <v>994</v>
+      </c>
+      <c r="E112">
+        <v>200</v>
+      </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>116</v>
       </c>
+      <c r="B113" t="s">
+        <v>995</v>
+      </c>
+      <c r="C113" t="s">
+        <v>996</v>
+      </c>
+      <c r="D113" t="s">
+        <v>997</v>
+      </c>
+      <c r="E113">
+        <v>200</v>
+      </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>117</v>
       </c>
+      <c r="B114" t="s">
+        <v>998</v>
+      </c>
+      <c r="C114" t="s">
+        <v>999</v>
+      </c>
+      <c r="D114" t="s">
+        <v>1000</v>
+      </c>
+      <c r="E114">
+        <v>200</v>
+      </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
@@ -4555,26 +5575,86 @@
       <c r="A134" t="s">
         <v>137</v>
       </c>
+      <c r="B134" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C134" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D134" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E134">
+        <v>200</v>
+      </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>138</v>
       </c>
+      <c r="B135" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C135" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D135" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E135">
+        <v>200</v>
+      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>139</v>
       </c>
+      <c r="B136" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C136" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D136" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E136">
+        <v>200</v>
+      </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>140</v>
       </c>
+      <c r="B137" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C137" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D137" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E137">
+        <v>200</v>
+      </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>141</v>
       </c>
+      <c r="B138" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C138" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D138" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E138">
+        <v>200</v>
+      </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
@@ -4795,26 +5875,86 @@
       <c r="A158" t="s">
         <v>161</v>
       </c>
+      <c r="B158" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C158" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D158" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E158">
+        <v>200</v>
+      </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>162</v>
       </c>
+      <c r="B159" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C159" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D159" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E159">
+        <v>200</v>
+      </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>163</v>
       </c>
+      <c r="B160" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C160" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D160" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E160">
+        <v>200</v>
+      </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>164</v>
       </c>
+      <c r="B161" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C161" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D161" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E161">
+        <v>200</v>
+      </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>165</v>
       </c>
+      <c r="B162" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C162" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D162" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E162">
+        <v>200</v>
+      </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
@@ -5035,26 +6175,86 @@
       <c r="A182" t="s">
         <v>185</v>
       </c>
+      <c r="B182" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C182" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D182" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E182">
+        <v>200</v>
+      </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>186</v>
       </c>
+      <c r="B183" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C183" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D183" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E183">
+        <v>200</v>
+      </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>187</v>
       </c>
+      <c r="B184" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C184" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D184" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E184">
+        <v>200</v>
+      </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>188</v>
       </c>
+      <c r="B185" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C185" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D185" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E185">
+        <v>200</v>
+      </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>189</v>
       </c>
+      <c r="B186" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C186" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D186" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E186">
+        <v>200</v>
+      </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
@@ -5275,26 +6475,86 @@
       <c r="A206" t="s">
         <v>209</v>
       </c>
+      <c r="B206" t="s">
+        <v>926</v>
+      </c>
+      <c r="C206" t="s">
+        <v>927</v>
+      </c>
+      <c r="D206" t="s">
+        <v>928</v>
+      </c>
+      <c r="E206">
+        <v>200</v>
+      </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>210</v>
       </c>
+      <c r="B207" t="s">
+        <v>929</v>
+      </c>
+      <c r="C207" t="s">
+        <v>930</v>
+      </c>
+      <c r="D207" t="s">
+        <v>931</v>
+      </c>
+      <c r="E207">
+        <v>200</v>
+      </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>211</v>
       </c>
+      <c r="B208" t="s">
+        <v>932</v>
+      </c>
+      <c r="C208" t="s">
+        <v>933</v>
+      </c>
+      <c r="D208" t="s">
+        <v>934</v>
+      </c>
+      <c r="E208">
+        <v>200</v>
+      </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>212</v>
       </c>
+      <c r="B209" t="s">
+        <v>935</v>
+      </c>
+      <c r="C209" t="s">
+        <v>936</v>
+      </c>
+      <c r="D209" t="s">
+        <v>937</v>
+      </c>
+      <c r="E209">
+        <v>200</v>
+      </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>213</v>
       </c>
+      <c r="B210" t="s">
+        <v>938</v>
+      </c>
+      <c r="C210" t="s">
+        <v>939</v>
+      </c>
+      <c r="D210" t="s">
+        <v>940</v>
+      </c>
+      <c r="E210">
+        <v>200</v>
+      </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
@@ -5515,26 +6775,86 @@
       <c r="A230" t="s">
         <v>233</v>
       </c>
+      <c r="B230" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C230" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D230" t="s">
+        <v>1048</v>
+      </c>
+      <c r="E230">
+        <v>200</v>
+      </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>234</v>
       </c>
+      <c r="B231" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C231" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D231" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E231">
+        <v>200</v>
+      </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>235</v>
       </c>
+      <c r="B232" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C232" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D232" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E232">
+        <v>200</v>
+      </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>236</v>
       </c>
+      <c r="B233" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C233" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D233" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E233">
+        <v>200</v>
+      </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>237</v>
       </c>
+      <c r="B234" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C234" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D234" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E234">
+        <v>200</v>
+      </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
@@ -5755,26 +7075,86 @@
       <c r="A254" t="s">
         <v>257</v>
       </c>
+      <c r="B254" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C254" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D254" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E254">
+        <v>200</v>
+      </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>258</v>
       </c>
+      <c r="B255" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C255" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D255" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E255">
+        <v>200</v>
+      </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>259</v>
       </c>
+      <c r="B256" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C256" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D256" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E256">
+        <v>200</v>
+      </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>260</v>
       </c>
+      <c r="B257" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C257" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D257" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E257">
+        <v>200</v>
+      </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>261</v>
       </c>
+      <c r="B258" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C258" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D258" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E258">
+        <v>200</v>
+      </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
@@ -5995,26 +7375,86 @@
       <c r="A278" t="s">
         <v>281</v>
       </c>
+      <c r="B278" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C278" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D278" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E278">
+        <v>200</v>
+      </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>282</v>
       </c>
+      <c r="B279" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C279" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D279" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E279">
+        <v>200</v>
+      </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>283</v>
       </c>
+      <c r="B280" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C280" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D280" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E280">
+        <v>200</v>
+      </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>284</v>
       </c>
+      <c r="B281" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C281" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D281" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E281">
+        <v>200</v>
+      </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>285</v>
       </c>
+      <c r="B282" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C282" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D282" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E282">
+        <v>200</v>
+      </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
@@ -6235,26 +7675,86 @@
       <c r="A302" t="s">
         <v>305</v>
       </c>
+      <c r="B302" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C302" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D302" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E302">
+        <v>200</v>
+      </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>306</v>
       </c>
+      <c r="B303" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C303" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D303" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E303">
+        <v>200</v>
+      </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>307</v>
       </c>
+      <c r="B304" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C304" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D304" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E304">
+        <v>200</v>
+      </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>308</v>
       </c>
+      <c r="B305" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C305" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D305" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E305">
+        <v>200</v>
+      </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>309</v>
       </c>
+      <c r="B306" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C306" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D306" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E306">
+        <v>200</v>
+      </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
@@ -6475,26 +7975,86 @@
       <c r="A326" t="s">
         <v>329</v>
       </c>
+      <c r="B326" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C326" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D326" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E326">
+        <v>200</v>
+      </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>330</v>
       </c>
+      <c r="B327" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C327" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D327" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E327">
+        <v>200</v>
+      </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>331</v>
       </c>
+      <c r="B328" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C328" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D328" t="s">
+        <v>1114</v>
+      </c>
+      <c r="E328">
+        <v>200</v>
+      </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>332</v>
       </c>
+      <c r="B329" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C329" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D329" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E329">
+        <v>200</v>
+      </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>333</v>
       </c>
+      <c r="B330" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C330" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D330" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E330">
+        <v>200</v>
+      </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
@@ -6715,26 +8275,86 @@
       <c r="A350" t="s">
         <v>353</v>
       </c>
+      <c r="B350" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C350" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D350" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E350">
+        <v>200</v>
+      </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>354</v>
       </c>
+      <c r="B351" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C351" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D351" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E351">
+        <v>200</v>
+      </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>355</v>
       </c>
+      <c r="B352" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C352" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D352" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E352">
+        <v>200</v>
+      </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>356</v>
       </c>
+      <c r="B353" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C353" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D353" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E353">
+        <v>200</v>
+      </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>357</v>
       </c>
+      <c r="B354" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C354" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D354" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E354">
+        <v>200</v>
+      </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
@@ -6955,25 +8575,85 @@
       <c r="A374" t="s">
         <v>377</v>
       </c>
+      <c r="B374" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C374" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D374" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E374">
+        <v>200</v>
+      </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>378</v>
       </c>
+      <c r="B375" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C375" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D375" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E375">
+        <v>200</v>
+      </c>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>379</v>
       </c>
+      <c r="B376" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C376" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D376" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E376">
+        <v>200</v>
+      </c>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>380</v>
       </c>
+      <c r="B377" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C377" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D377" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E377">
+        <v>200</v>
+      </c>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>381</v>
+      </c>
+      <c r="B378" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C378" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D378" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E378">
+        <v>200</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.2">
@@ -7021,14 +8701,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="25.6640625" customWidth="1"/>
     <col min="6" max="6" width="5.6640625" customWidth="1"/>
     <col min="7" max="11" width="26.6640625" customWidth="1"/>
-    <col min="12" max="24" width="5.6640625" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" customWidth="1"/>
+    <col min="14" max="17" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
@@ -7142,6 +8828,21 @@
       <c r="L2" s="2" t="s">
         <v>398</v>
       </c>
+      <c r="N2" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>923</v>
+      </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -7177,6 +8878,21 @@
       <c r="L3" t="s">
         <v>408</v>
       </c>
+      <c r="N3" t="s">
+        <v>941</v>
+      </c>
+      <c r="O3" t="s">
+        <v>944</v>
+      </c>
+      <c r="P3" t="s">
+        <v>947</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>950</v>
+      </c>
+      <c r="R3" t="s">
+        <v>953</v>
+      </c>
     </row>
     <row r="4" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -7212,6 +8928,21 @@
       <c r="L4" s="2" t="s">
         <v>418</v>
       </c>
+      <c r="N4" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>968</v>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -7247,6 +8978,21 @@
       <c r="L5" t="s">
         <v>428</v>
       </c>
+      <c r="N5" t="s">
+        <v>971</v>
+      </c>
+      <c r="O5" t="s">
+        <v>974</v>
+      </c>
+      <c r="P5" t="s">
+        <v>977</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>980</v>
+      </c>
+      <c r="R5" t="s">
+        <v>983</v>
+      </c>
     </row>
     <row r="6" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -7282,6 +9028,21 @@
       <c r="L6" s="2" t="s">
         <v>438</v>
       </c>
+      <c r="N6" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>989</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>998</v>
+      </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -7317,6 +9078,21 @@
       <c r="L7" t="s">
         <v>448</v>
       </c>
+      <c r="N7" t="s">
+        <v>1001</v>
+      </c>
+      <c r="O7" t="s">
+        <v>1004</v>
+      </c>
+      <c r="P7" t="s">
+        <v>1007</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>1010</v>
+      </c>
+      <c r="R7" t="s">
+        <v>1013</v>
+      </c>
     </row>
     <row r="8" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -7352,6 +9128,21 @@
       <c r="L8" s="2" t="s">
         <v>458</v>
       </c>
+      <c r="N8" s="2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>1025</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>1028</v>
+      </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -7387,6 +9178,21 @@
       <c r="L9" t="s">
         <v>468</v>
       </c>
+      <c r="N9" t="s">
+        <v>1031</v>
+      </c>
+      <c r="O9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="P9" t="s">
+        <v>1037</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>1040</v>
+      </c>
+      <c r="R9" t="s">
+        <v>1043</v>
+      </c>
     </row>
     <row r="10" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -7422,6 +9228,21 @@
       <c r="L10" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="N10" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>938</v>
+      </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -7457,6 +9278,21 @@
       <c r="L11" t="s">
         <v>488</v>
       </c>
+      <c r="N11" t="s">
+        <v>1046</v>
+      </c>
+      <c r="O11" t="s">
+        <v>1049</v>
+      </c>
+      <c r="P11" t="s">
+        <v>1052</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>1055</v>
+      </c>
+      <c r="R11" t="s">
+        <v>1058</v>
+      </c>
     </row>
     <row r="12" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -7492,6 +9328,21 @@
       <c r="L12" s="2" t="s">
         <v>498</v>
       </c>
+      <c r="N12" s="2" t="s">
+        <v>1061</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>1067</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>1070</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>1073</v>
+      </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -7527,6 +9378,21 @@
       <c r="L13" t="s">
         <v>508</v>
       </c>
+      <c r="N13" t="s">
+        <v>1076</v>
+      </c>
+      <c r="O13" t="s">
+        <v>1079</v>
+      </c>
+      <c r="P13" t="s">
+        <v>1082</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>1085</v>
+      </c>
+      <c r="R13" t="s">
+        <v>1088</v>
+      </c>
     </row>
     <row r="14" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -7562,6 +9428,21 @@
       <c r="L14" s="2" t="s">
         <v>518</v>
       </c>
+      <c r="N14" s="2" t="s">
+        <v>1091</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>1094</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>1097</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>1100</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>1103</v>
+      </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -7597,6 +9478,21 @@
       <c r="L15" t="s">
         <v>528</v>
       </c>
+      <c r="N15" t="s">
+        <v>1106</v>
+      </c>
+      <c r="O15" t="s">
+        <v>1109</v>
+      </c>
+      <c r="P15" t="s">
+        <v>1112</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>1115</v>
+      </c>
+      <c r="R15" t="s">
+        <v>1118</v>
+      </c>
     </row>
     <row r="16" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -7632,8 +9528,23 @@
       <c r="L16" s="2" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N16" s="2" t="s">
+        <v>1121</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>1124</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>909</v>
       </c>
@@ -7666,6 +9577,21 @@
       </c>
       <c r="L17" t="s">
         <v>548</v>
+      </c>
+      <c r="N17" t="s">
+        <v>1136</v>
+      </c>
+      <c r="O17" t="s">
+        <v>1139</v>
+      </c>
+      <c r="P17" t="s">
+        <v>1142</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>1145</v>
+      </c>
+      <c r="R17" t="s">
+        <v>1148</v>
       </c>
     </row>
   </sheetData>
@@ -7677,7 +9603,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7799,6 +9727,21 @@
       <c r="L2" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N2" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -7834,6 +9777,21 @@
       <c r="L3" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N3" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -7869,6 +9827,21 @@
       <c r="L4" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N4" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -7904,6 +9877,21 @@
       <c r="L5" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N5" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -7939,6 +9927,21 @@
       <c r="L6" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N6" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -7974,6 +9977,21 @@
       <c r="L7" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N7" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -8009,6 +10027,21 @@
       <c r="L8" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N8" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -8044,6 +10077,21 @@
       <c r="L9" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N9" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -8079,6 +10127,21 @@
       <c r="L10" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N10" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -8114,6 +10177,21 @@
       <c r="L11" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N11" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -8149,6 +10227,21 @@
       <c r="L12" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N12" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -8184,6 +10277,21 @@
       <c r="L13" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N13" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -8219,6 +10327,21 @@
       <c r="L14" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N14" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -8254,6 +10377,21 @@
       <c r="L15" s="3" t="s">
         <v>910</v>
       </c>
+      <c r="N15" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -8289,8 +10427,23 @@
       <c r="L16" s="3" t="s">
         <v>910</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N16" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>909</v>
       </c>
@@ -8322,6 +10475,21 @@
         <v>910</v>
       </c>
       <c r="L17" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R17" s="3" t="s">
         <v>910</v>
       </c>
     </row>

</xml_diff>